<commit_message>
Gantt chart initial time estimations
</commit_message>
<xml_diff>
--- a/Gantt_Chart.xlsx
+++ b/Gantt_Chart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riovi\Documents\School\SeniorYear\SoftwareEngineering\BlackjackHolder\blackjackSoftwareEngineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareEngineering\BlackjackHolder\blackjackSoftwareEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E26CCBB-3698-473B-8847-26DACC1A460B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{2BAB2DE8-7B2B-43F2-A8BF-C7DE75B453B6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Task</t>
   </si>
@@ -60,22 +60,25 @@
     <t>Bet Functionality</t>
   </si>
   <si>
-    <t>Unit Testing</t>
-  </si>
-  <si>
-    <t>Integration Testing</t>
-  </si>
-  <si>
-    <t>Final Testing</t>
-  </si>
-  <si>
-    <t>Start Game GUI and functionality</t>
+    <t>Integrate old Lab Work (GJ)</t>
+  </si>
+  <si>
+    <t>Start Game GUI and functionality (AJ)</t>
+  </si>
+  <si>
+    <t>Unit Testing (all)</t>
+  </si>
+  <si>
+    <t>Integration Testing (all)</t>
+  </si>
+  <si>
+    <t>Final Testing (all)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,16 +424,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B655D0C6-DCD1-4D23-BE6F-6163A97CC453}">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="44" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="4" width="19.42578125" customWidth="1"/>
   </cols>
@@ -447,65 +451,152 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43410</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43412</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43412</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43412</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43412</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
+      <c r="B7" s="1">
+        <v>43412</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43412</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43414</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43416</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43416</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43425</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43428</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>43433</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C13">
+    <sortCondition ref="B2:B13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final work on Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt_Chart.xlsx
+++ b/Gantt_Chart.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftwareEngineering\BlackjackHolder\blackjackSoftwareEngineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riovi\Documents\School\SeniorYear\SoftwareEngineering\BlackjackHolder\blackjackSoftwareEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB03FFE-91FC-4B30-8E8C-B9D6E5A6FCF7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Task</t>
   </si>
@@ -34,30 +34,6 @@
   </si>
   <si>
     <t>Days to Complete</t>
-  </si>
-  <si>
-    <t>Client GUI</t>
-  </si>
-  <si>
-    <t>Server GUI</t>
-  </si>
-  <si>
-    <t>Gameplay GUI</t>
-  </si>
-  <si>
-    <t>Database Creation</t>
-  </si>
-  <si>
-    <t>Database Communication</t>
-  </si>
-  <si>
-    <t>Gameplay Functionality</t>
-  </si>
-  <si>
-    <t>Bet GUI</t>
-  </si>
-  <si>
-    <t>Bet Functionality</t>
   </si>
   <si>
     <t>Integrate old Lab Work (GJ)</t>
@@ -74,11 +50,38 @@
   <si>
     <t>Final Testing (all)</t>
   </si>
+  <si>
+    <t>Server GUI (GJ)</t>
+  </si>
+  <si>
+    <t>Database Creation (MK)</t>
+  </si>
+  <si>
+    <t>Database Communication (MK)</t>
+  </si>
+  <si>
+    <t>Gameplay GUI (MD)</t>
+  </si>
+  <si>
+    <t>Gameplay Functionality (data/control) (MD)</t>
+  </si>
+  <si>
+    <t>Bet GUI (AJ)</t>
+  </si>
+  <si>
+    <t>Bet Functionality (data/control) (GJ)</t>
+  </si>
+  <si>
+    <t>Client GUI (GJ)</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,6 +129,1034 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Integrate old Lab Work (GJ)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Client GUI (GJ)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Server GUI (GJ)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Start Game GUI and functionality (AJ)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Gameplay GUI (MD)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bet GUI (AJ)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Database Creation (MK)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Database Communication (MK)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Gameplay Functionality (data/control) (MD)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Bet Functionality (data/control) (GJ)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Unit Testing (all)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Integration Testing (all)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Final Testing (all)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43412</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43412</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43412</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43412</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43412</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43414</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43425</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43428</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43433</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4117-4238-B172-B23131CC71A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Days to Complete</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Integrate old Lab Work (GJ)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Client GUI (GJ)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Server GUI (GJ)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Start Game GUI and functionality (AJ)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Gameplay GUI (MD)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bet GUI (AJ)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Database Creation (MK)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Database Communication (MK)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Gameplay Functionality (data/control) (MD)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Bet Functionality (data/control) (GJ)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Unit Testing (all)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Integration Testing (all)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Final Testing (all)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4117-4238-B172-B23131CC71A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="697224464"/>
+        <c:axId val="697269408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="697224464"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="697269408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="697269408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="43405"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="697224464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2162174</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDBDAC32-5D80-45EE-B6AB-15E9ACBE982D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -424,21 +1455,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="4" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,10 +1485,13 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>43410</v>
@@ -459,10 +1499,14 @@
       <c r="C2">
         <v>2</v>
       </c>
+      <c r="D2" s="1">
+        <f>B2+C2</f>
+        <v>43412</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>43412</v>
@@ -470,10 +1514,14 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D14" si="0">B3+C3</f>
+        <v>43414</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>43412</v>
@@ -481,10 +1529,14 @@
       <c r="C4">
         <v>2</v>
       </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>43414</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>43412</v>
@@ -492,10 +1544,14 @@
       <c r="C5">
         <v>2</v>
       </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>43414</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>43412</v>
@@ -503,10 +1559,14 @@
       <c r="C6">
         <v>4</v>
       </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>43416</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>43412</v>
@@ -514,10 +1574,14 @@
       <c r="C7">
         <v>4</v>
       </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>43416</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>43412</v>
@@ -525,10 +1589,14 @@
       <c r="C8">
         <v>2</v>
       </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>43414</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>43414</v>
@@ -536,10 +1604,14 @@
       <c r="C9">
         <v>4</v>
       </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>43418</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>43416</v>
@@ -547,10 +1619,14 @@
       <c r="C10">
         <v>9</v>
       </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>43425</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
         <v>43416</v>
@@ -558,10 +1634,14 @@
       <c r="C11">
         <v>8</v>
       </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>43424</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
         <v>43425</v>
@@ -569,10 +1649,14 @@
       <c r="C12">
         <v>3</v>
       </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>43428</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>43428</v>
@@ -580,16 +1664,24 @@
       <c r="C13">
         <v>5</v>
       </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>43433</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1">
         <v>43433</v>
       </c>
       <c r="C14">
         <v>4</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>43437</v>
       </c>
     </row>
   </sheetData>
@@ -598,5 +1690,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>